<commit_message>
Cleanup project structure and added updated budgeting and presentation
</commit_message>
<xml_diff>
--- a/business values/budget.xlsx
+++ b/business values/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pakr\Documents\My projects\BV\business values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F23272-CC30-4F4D-95F4-51EA30BC76AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C54B16-F50F-49EB-AD58-AAB6968791E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salary estimations" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>Position</t>
   </si>
@@ -106,15 +106,9 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Customers, end of the month</t>
-  </si>
-  <si>
     <t>Subscriptions</t>
   </si>
   <si>
-    <t>Subscription monthly churn rate</t>
-  </si>
-  <si>
     <t>Total yearly pay</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>VAT</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>Corporate tax</t>
   </si>
   <si>
@@ -179,6 +170,12 @@
   </si>
   <si>
     <t>Personal profit</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>Customers</t>
   </si>
 </sst>
 </file>
@@ -332,7 +329,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Income!$H$6:$H$16</c:f>
+              <c:f>Income!$G$6:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -340,34 +337,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640</c:v>
+                  <c:v>1280</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2006</c:v>
+                  <c:v>3922</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4588</c:v>
+                  <c:v>8996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9752</c:v>
+                  <c:v>19144</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20080</c:v>
+                  <c:v>39440</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40736</c:v>
+                  <c:v>80032</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>73088</c:v>
+                  <c:v>130496</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>117388</c:v>
+                  <c:v>187856</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>170308</c:v>
+                  <c:v>252471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>227918</c:v>
+                  <c:v>323724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -399,42 +396,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Income!$I$6:$I$16</c:f>
+              <c:f>Income!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>54000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57000</c:v>
+                  <c:v>63000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60000</c:v>
+                  <c:v>66000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>63000</c:v>
+                  <c:v>69000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>66000</c:v>
+                  <c:v>72000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69000</c:v>
+                  <c:v>75000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72000</c:v>
+                  <c:v>78000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75000</c:v>
+                  <c:v>81000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>78000</c:v>
+                  <c:v>84000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>81000</c:v>
+                  <c:v>87000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>84000</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -466,42 +463,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Income!$O$6:$O$16</c:f>
+              <c:f>Income!$M$6:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-54000</c:v>
+                  <c:v>-60000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-56360</c:v>
+                  <c:v>-61720</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-57994</c:v>
+                  <c:v>-62078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-58412</c:v>
+                  <c:v>-60004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-56248</c:v>
+                  <c:v>-52856</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-48920</c:v>
+                  <c:v>-35560</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-31264</c:v>
+                  <c:v>1152.144</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1912</c:v>
+                  <c:v>28064.232000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22332.995999999999</c:v>
+                  <c:v>58886.351999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50637.635999999999</c:v>
+                  <c:v>93822.057000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>81601.505999999994</c:v>
+                  <c:v>132521.508</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,81 +803,81 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Income!$Q$6:$Q$29</c:f>
+              <c:f>Income!$N$6:$N$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>-211500</c:v>
+                  <c:v>-217500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-240110</c:v>
+                  <c:v>-245470</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-267994</c:v>
+                  <c:v>-272078</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-294662</c:v>
+                  <c:v>-296254</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-318748</c:v>
+                  <c:v>-315356</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-337670</c:v>
+                  <c:v>-324310</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-346264</c:v>
+                  <c:v>-313847.85600000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-343162</c:v>
+                  <c:v>-313185.76799999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-345167.00400000002</c:v>
+                  <c:v>-308613.64799999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-343112.364</c:v>
+                  <c:v>-299927.94299999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-338398.49400000001</c:v>
+                  <c:v>-287478.49199999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-329029.554</c:v>
+                  <c:v>-271895.23200000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-316150.88399999996</c:v>
+                  <c:v>-253165.12200000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-303266.54399999999</c:v>
+                  <c:v>-234004.092</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-284281.28399999999</c:v>
+                  <c:v>-208742.14199999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-262030.10399999999</c:v>
+                  <c:v>-180214.272</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-236513.00399999996</c:v>
+                  <c:v>-148420.48199999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-207729.984</c:v>
+                  <c:v>-113360.772</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-175681.04399999999</c:v>
+                  <c:v>-75035.141999999993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-140366.18400000001</c:v>
+                  <c:v>-33443.591999999946</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-101785.40399999998</c:v>
+                  <c:v>11413.878000000026</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-59938.703999999911</c:v>
+                  <c:v>59537.267999999924</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-14826.084000000032</c:v>
+                  <c:v>110926.57799999998</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>33552.456000000006</c:v>
+                  <c:v>165581.80799999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2184,7 +2181,7 @@
       <xdr:rowOff>27384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>1089422</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>103584</xdr:rowOff>
@@ -2214,13 +2211,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>952501</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>146446</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1214439</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>32146</xdr:rowOff>
@@ -2516,19 +2513,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2539,10 +2536,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2557,7 +2554,7 @@
         <v>315000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2568,7 +2565,7 @@
         <v>83382.91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2579,7 +2576,7 @@
         <v>72202.91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2590,7 +2587,7 @@
         <v>60312.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2611,27 +2608,27 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="6" max="7" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="6" max="7" width="22.33203125" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2645,7 +2642,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2660,7 +2657,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2675,9 +2672,9 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>5000</v>
@@ -2689,9 +2686,9 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>24000</v>
@@ -2703,46 +2700,46 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>25000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>12000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>10000</v>
@@ -2755,32 +2752,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0817564C-7C63-4B82-9CEC-2BCF9626B39E}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" customWidth="1"/>
-    <col min="10" max="10" width="28.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
-    <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="17.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" customWidth="1"/>
+    <col min="14" max="14" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -2796,17 +2792,14 @@
       <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -2817,22 +2810,19 @@
         <v>12345</v>
       </c>
       <c r="E2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
         <v>0.04</v>
       </c>
-      <c r="G2">
-        <v>0.1</v>
+      <c r="H2">
+        <v>3000</v>
       </c>
       <c r="I2">
-        <v>3000</v>
-      </c>
-      <c r="J2">
         <v>26250</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -2840,48 +2830,48 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
       </c>
       <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
         <v>42</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>43</v>
       </c>
-      <c r="N5" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2897,1229 +2887,1229 @@
       <c r="F6">
         <v>0</v>
       </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
       <c r="H6">
+        <v>60000</v>
+      </c>
+      <c r="I6">
+        <f>I2*6</f>
+        <v>157500</v>
+      </c>
+      <c r="J6">
+        <f>(G6-H6)*0.19</f>
+        <v>-11400</v>
+      </c>
+      <c r="K6">
+        <f>G6-H6-IF(J6&gt;0,J6,0)</f>
+        <v>-60000</v>
+      </c>
+      <c r="L6">
+        <f>MAX(K6,0)*0.3</f>
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>54000</v>
-      </c>
-      <c r="J6">
-        <f>J2*6</f>
-        <v>157500</v>
-      </c>
-      <c r="L6">
-        <f>(H6-I6)*0.19</f>
-        <v>-10260</v>
-      </c>
       <c r="M6">
-        <f>H6-I6-IF(L6&gt;0,L6,0)</f>
-        <v>-54000</v>
+        <f>K6-L6</f>
+        <v>-60000</v>
       </c>
       <c r="N6">
-        <f>MAX(M6,0)*0.3</f>
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <f>M6-N6</f>
-        <v>-54000</v>
-      </c>
-      <c r="Q6">
-        <f>O6-J6</f>
-        <v>-211500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M6-I6</f>
+        <v>-217500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="E7">
         <f>$B$2*40*(B7-C7)</f>
-        <v>640</v>
+        <v>1280</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7">
+        <f>SUM(E$7:E7,F$7:F7)</f>
+        <v>1280</v>
+      </c>
       <c r="H7">
-        <f>SUM(E$7:E7,F$7:F7)</f>
-        <v>640</v>
+        <f>H6+H$2</f>
+        <v>63000</v>
       </c>
       <c r="I7">
-        <f>I6+I$2</f>
-        <v>57000</v>
+        <f>I6+$I$2</f>
+        <v>183750</v>
       </c>
       <c r="J7">
-        <f>J6+$J$2</f>
-        <v>183750</v>
+        <f>(G7-H7)*0.19</f>
+        <v>-11726.8</v>
+      </c>
+      <c r="K7">
+        <f>G7-H7-IF(J7&gt;0,J7,0)</f>
+        <v>-61720</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L29" si="0">(H7-I7)*0.19</f>
-        <v>-10708.4</v>
+        <f t="shared" ref="L7:L29" si="0">MAX(K7,0)*0.3</f>
+        <v>0</v>
       </c>
       <c r="M7">
-        <f t="shared" ref="M7:M29" si="1">H7-I7-IF(L7&gt;0,L7,0)</f>
-        <v>-56360</v>
+        <f t="shared" ref="M7:M29" si="1">K7-L7</f>
+        <v>-61720</v>
       </c>
       <c r="N7">
-        <f t="shared" ref="N7:N29" si="2">MAX(M7,0)*0.3</f>
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <f t="shared" ref="O7:O29" si="3">M7-N7</f>
-        <v>-56360</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" ref="Q7:Q29" si="4">O7-J7</f>
-        <v>-240110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M7-I7</f>
+        <v>-245470</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="C8">
         <f>B7*0.1</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E29" si="5">$B$2*40*(B8-C8)</f>
-        <v>1216</v>
+        <f t="shared" ref="E8:E29" si="2">$B$2*40*(B8-C8)</f>
+        <v>2432</v>
       </c>
       <c r="F8">
-        <f>(C8-C7)*$B$3</f>
-        <v>150</v>
+        <f>(C8-C7)*$B$3*0.7</f>
+        <v>210</v>
+      </c>
+      <c r="G8">
+        <f>SUM(E$7:E8,F$7:F8)</f>
+        <v>3922</v>
       </c>
       <c r="H8">
-        <f>SUM(E$7:E8,F$7:F8)</f>
-        <v>2006</v>
+        <f t="shared" ref="H8:H29" si="3">H7+H$2</f>
+        <v>66000</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I29" si="6">I7+I$2</f>
-        <v>60000</v>
+        <f t="shared" ref="I8:I29" si="4">I7+$I$2</f>
+        <v>210000</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J29" si="7">J7+$J$2</f>
-        <v>210000</v>
+        <f>(G8-H8)*0.19</f>
+        <v>-11794.82</v>
+      </c>
+      <c r="K8">
+        <f>G8-H8-IF(J8&gt;0,J8,0)</f>
+        <v>-62078</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>-11018.86</v>
+        <v>0</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>-57994</v>
+        <v>-62078</v>
       </c>
       <c r="N8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="3"/>
-        <v>-57994</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>-267994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M8-I8</f>
+        <v>-272078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9">
-        <v>400</v>
+        <v>800</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:C29" si="8">B8*0.1</f>
-        <v>20</v>
+        <f t="shared" ref="C9:C29" si="5">B8*0.1</f>
+        <v>40</v>
       </c>
       <c r="E9">
-        <f t="shared" si="5"/>
-        <v>2432</v>
+        <f t="shared" si="2"/>
+        <v>4864</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F29" si="9">(C9-C8)*$B$3</f>
-        <v>150</v>
+        <f t="shared" ref="F9:F29" si="6">(C9-C8)*$B$3*0.7</f>
+        <v>210</v>
+      </c>
+      <c r="G9">
+        <f>SUM(E$7:E9,F$7:F9)</f>
+        <v>8996</v>
       </c>
       <c r="H9">
-        <f>SUM(E$7:E9,F$7:F9)</f>
-        <v>4588</v>
+        <f t="shared" si="3"/>
+        <v>69000</v>
       </c>
       <c r="I9">
-        <f t="shared" si="6"/>
-        <v>63000</v>
+        <f t="shared" si="4"/>
+        <v>236250</v>
       </c>
       <c r="J9">
-        <f t="shared" si="7"/>
-        <v>236250</v>
+        <f>(G9-H9)*0.19</f>
+        <v>-11400.76</v>
+      </c>
+      <c r="K9">
+        <f>G9-H9-IF(J9&gt;0,J9,0)</f>
+        <v>-60004</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>-11098.28</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>-58412</v>
+        <v>-60004</v>
       </c>
       <c r="N9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="3"/>
-        <v>-58412</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="4"/>
-        <v>-294662</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M9-I9</f>
+        <v>-296254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="C10">
-        <f t="shared" si="8"/>
-        <v>40</v>
+        <f t="shared" si="5"/>
+        <v>80</v>
       </c>
       <c r="E10">
-        <f t="shared" si="5"/>
-        <v>4864</v>
+        <f t="shared" si="2"/>
+        <v>9728</v>
       </c>
       <c r="F10">
-        <f t="shared" si="9"/>
-        <v>300</v>
+        <f t="shared" si="6"/>
+        <v>420</v>
+      </c>
+      <c r="G10">
+        <f>SUM(E$7:E10,F$7:F10)</f>
+        <v>19144</v>
       </c>
       <c r="H10">
-        <f>SUM(E$7:E10,F$7:F10)</f>
-        <v>9752</v>
+        <f t="shared" si="3"/>
+        <v>72000</v>
       </c>
       <c r="I10">
-        <f t="shared" si="6"/>
-        <v>66000</v>
+        <f t="shared" si="4"/>
+        <v>262500</v>
       </c>
       <c r="J10">
-        <f t="shared" si="7"/>
-        <v>262500</v>
+        <f>(G10-H10)*0.19</f>
+        <v>-10042.64</v>
+      </c>
+      <c r="K10">
+        <f>G10-H10-IF(J10&gt;0,J10,0)</f>
+        <v>-52856</v>
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>-10687.12</v>
+        <v>0</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>-56248</v>
+        <v>-52856</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="3"/>
-        <v>-56248</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="4"/>
-        <v>-318748</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M10-I10</f>
+        <v>-315356</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11">
-        <v>1600</v>
+        <v>3200</v>
       </c>
       <c r="C11">
-        <f t="shared" si="8"/>
-        <v>80</v>
+        <f t="shared" si="5"/>
+        <v>160</v>
       </c>
       <c r="E11">
-        <f t="shared" si="5"/>
-        <v>9728</v>
+        <f t="shared" si="2"/>
+        <v>19456</v>
       </c>
       <c r="F11">
-        <f t="shared" si="9"/>
-        <v>600</v>
+        <f t="shared" si="6"/>
+        <v>840</v>
+      </c>
+      <c r="G11">
+        <f>SUM(E$7:E11,F$7:F11)</f>
+        <v>39440</v>
       </c>
       <c r="H11">
-        <f>SUM(E$7:E11,F$7:F11)</f>
-        <v>20080</v>
+        <f t="shared" si="3"/>
+        <v>75000</v>
       </c>
       <c r="I11">
-        <f t="shared" si="6"/>
-        <v>69000</v>
+        <f t="shared" si="4"/>
+        <v>288750</v>
       </c>
       <c r="J11">
-        <f t="shared" si="7"/>
-        <v>288750</v>
+        <f>(G11-H11)*0.19</f>
+        <v>-6756.4</v>
+      </c>
+      <c r="K11">
+        <f>G11-H11-IF(J11&gt;0,J11,0)</f>
+        <v>-35560</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>-9294.7999999999993</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>-48920</v>
+        <v>-35560</v>
       </c>
       <c r="N11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="3"/>
-        <v>-48920</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="4"/>
-        <v>-337670</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M11-I11</f>
+        <v>-324310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12">
-        <v>3200</v>
+        <v>6400</v>
       </c>
       <c r="C12">
-        <f t="shared" si="8"/>
-        <v>160</v>
+        <f t="shared" si="5"/>
+        <v>320</v>
       </c>
       <c r="E12">
-        <f t="shared" si="5"/>
-        <v>19456</v>
+        <f t="shared" si="2"/>
+        <v>38912</v>
       </c>
       <c r="F12">
-        <f t="shared" si="9"/>
-        <v>1200</v>
+        <f t="shared" si="6"/>
+        <v>1680</v>
+      </c>
+      <c r="G12">
+        <f>SUM(E$7:E12,F$7:F12)</f>
+        <v>80032</v>
       </c>
       <c r="H12">
-        <f>SUM(E$7:E12,F$7:F12)</f>
-        <v>40736</v>
+        <f t="shared" si="3"/>
+        <v>78000</v>
       </c>
       <c r="I12">
-        <f t="shared" si="6"/>
-        <v>72000</v>
+        <f t="shared" si="4"/>
+        <v>315000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="7"/>
-        <v>315000</v>
+        <f>(G12-H12)*0.19</f>
+        <v>386.08</v>
+      </c>
+      <c r="K12">
+        <f>G12-H12-IF(J12&gt;0,J12,0)</f>
+        <v>1645.92</v>
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>-5940.16</v>
+        <v>493.77600000000001</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>-31264</v>
+        <v>1152.144</v>
       </c>
       <c r="N12">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="3"/>
-        <v>-31264</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="4"/>
-        <v>-346264</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M12-I12</f>
+        <v>-313847.85600000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="C13">
-        <f t="shared" si="8"/>
-        <v>320</v>
+        <f t="shared" si="5"/>
+        <v>640</v>
       </c>
       <c r="E13">
-        <f t="shared" si="5"/>
-        <v>29952</v>
+        <f t="shared" si="2"/>
+        <v>47104</v>
       </c>
       <c r="F13">
-        <f t="shared" si="9"/>
-        <v>2400</v>
+        <f t="shared" si="6"/>
+        <v>3360</v>
+      </c>
+      <c r="G13">
+        <f>SUM(E$7:E13,F$7:F13)</f>
+        <v>130496</v>
       </c>
       <c r="H13">
-        <f>SUM(E$7:E13,F$7:F13)</f>
-        <v>73088</v>
+        <f t="shared" si="3"/>
+        <v>81000</v>
       </c>
       <c r="I13">
-        <f t="shared" si="6"/>
-        <v>75000</v>
+        <f t="shared" si="4"/>
+        <v>341250</v>
       </c>
       <c r="J13">
-        <f t="shared" si="7"/>
-        <v>341250</v>
+        <f>(G13-H13)*0.19</f>
+        <v>9404.24</v>
+      </c>
+      <c r="K13">
+        <f>G13-H13-IF(J13&gt;0,J13,0)</f>
+        <v>40091.760000000002</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>-363.28000000000003</v>
+        <v>12027.528</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>-1912</v>
+        <v>28064.232000000004</v>
       </c>
       <c r="N13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="3"/>
-        <v>-1912</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="4"/>
-        <v>-343162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M13-I13</f>
+        <v>-313185.76799999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14">
-        <v>7000</v>
+        <v>9500</v>
       </c>
       <c r="C14">
-        <f t="shared" si="8"/>
-        <v>500</v>
+        <f t="shared" si="5"/>
+        <v>800</v>
       </c>
       <c r="E14">
-        <f t="shared" si="5"/>
-        <v>41600</v>
+        <f t="shared" si="2"/>
+        <v>55680</v>
       </c>
       <c r="F14">
-        <f t="shared" si="9"/>
-        <v>2700</v>
+        <f t="shared" si="6"/>
+        <v>1680</v>
+      </c>
+      <c r="G14">
+        <f>SUM(E$7:E14,F$7:F14)</f>
+        <v>187856</v>
       </c>
       <c r="H14">
-        <f>SUM(E$7:E14,F$7:F14)</f>
-        <v>117388</v>
+        <f t="shared" si="3"/>
+        <v>84000</v>
       </c>
       <c r="I14">
-        <f t="shared" si="6"/>
-        <v>78000</v>
+        <f t="shared" si="4"/>
+        <v>367500</v>
       </c>
       <c r="J14">
-        <f t="shared" si="7"/>
-        <v>367500</v>
+        <f>(G14-H14)*0.19</f>
+        <v>19732.64</v>
+      </c>
+      <c r="K14">
+        <f>G14-H14-IF(J14&gt;0,J14,0)</f>
+        <v>84123.36</v>
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>7483.72</v>
+        <v>25237.007999999998</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>31904.28</v>
+        <v>58886.351999999999</v>
       </c>
       <c r="N14">
-        <f t="shared" si="2"/>
-        <v>9571.2839999999997</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="3"/>
-        <v>22332.995999999999</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="4"/>
-        <v>-345167.00400000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M14-I14</f>
+        <v>-308613.64799999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15">
-        <v>8500</v>
+        <v>10800</v>
       </c>
       <c r="C15">
-        <f t="shared" si="8"/>
-        <v>700</v>
+        <f t="shared" si="5"/>
+        <v>950</v>
       </c>
       <c r="E15">
-        <f t="shared" si="5"/>
-        <v>49920</v>
+        <f t="shared" si="2"/>
+        <v>63040</v>
       </c>
       <c r="F15">
-        <f t="shared" si="9"/>
-        <v>3000</v>
+        <f t="shared" si="6"/>
+        <v>1575</v>
+      </c>
+      <c r="G15">
+        <f>SUM(E$7:E15,F$7:F15)</f>
+        <v>252471</v>
       </c>
       <c r="H15">
-        <f>SUM(E$7:E15,F$7:F15)</f>
-        <v>170308</v>
+        <f t="shared" si="3"/>
+        <v>87000</v>
       </c>
       <c r="I15">
-        <f t="shared" si="6"/>
-        <v>81000</v>
+        <f t="shared" si="4"/>
+        <v>393750</v>
       </c>
       <c r="J15">
-        <f t="shared" si="7"/>
-        <v>393750</v>
+        <f>(G15-H15)*0.19</f>
+        <v>31439.49</v>
+      </c>
+      <c r="K15">
+        <f>G15-H15-IF(J15&gt;0,J15,0)</f>
+        <v>134031.51</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>16968.52</v>
+        <v>40209.453000000001</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>72339.48</v>
+        <v>93822.057000000001</v>
       </c>
       <c r="N15">
-        <f t="shared" si="2"/>
-        <v>21701.843999999997</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="3"/>
-        <v>50637.635999999999</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="4"/>
-        <v>-343112.364</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M15-I15</f>
+        <v>-299927.94299999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16">
-        <v>9500</v>
+        <v>12000</v>
       </c>
       <c r="C16">
-        <f t="shared" si="8"/>
-        <v>850</v>
+        <f t="shared" si="5"/>
+        <v>1080</v>
       </c>
       <c r="E16">
-        <f t="shared" si="5"/>
-        <v>55360</v>
+        <f t="shared" si="2"/>
+        <v>69888</v>
       </c>
       <c r="F16">
-        <f t="shared" si="9"/>
-        <v>2250</v>
+        <f t="shared" si="6"/>
+        <v>1365</v>
+      </c>
+      <c r="G16">
+        <f>SUM(E$7:E16,F$7:F16)</f>
+        <v>323724</v>
       </c>
       <c r="H16">
-        <f>SUM(E$7:E16,F$7:F16)</f>
-        <v>227918</v>
+        <f t="shared" si="3"/>
+        <v>90000</v>
       </c>
       <c r="I16">
-        <f t="shared" si="6"/>
-        <v>84000</v>
+        <f t="shared" si="4"/>
+        <v>420000</v>
       </c>
       <c r="J16">
-        <f t="shared" si="7"/>
-        <v>420000</v>
+        <f>(G16-H16)*0.19</f>
+        <v>44407.56</v>
+      </c>
+      <c r="K16">
+        <f>G16-H16-IF(J16&gt;0,J16,0)</f>
+        <v>189316.44</v>
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>27344.420000000002</v>
+        <v>56794.932000000001</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>116573.58</v>
+        <v>132521.508</v>
       </c>
       <c r="N16">
-        <f t="shared" si="2"/>
-        <v>34972.074000000001</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="3"/>
-        <v>81601.505999999994</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="4"/>
-        <v>-338398.49400000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M16-I16</f>
+        <v>-287478.49199999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17">
-        <v>11000</v>
+        <v>13000</v>
       </c>
       <c r="C17">
-        <f t="shared" si="8"/>
-        <v>950</v>
+        <f t="shared" si="5"/>
+        <v>1200</v>
       </c>
       <c r="E17">
-        <f t="shared" si="5"/>
-        <v>64320</v>
+        <f t="shared" si="2"/>
+        <v>75520</v>
       </c>
       <c r="F17">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1260</v>
+      </c>
+      <c r="G17">
+        <f>SUM(E$7:E17,F$7:F17)</f>
+        <v>400504</v>
       </c>
       <c r="H17">
-        <f>SUM(E$7:E17,F$7:F17)</f>
-        <v>293738</v>
+        <f t="shared" si="3"/>
+        <v>93000</v>
       </c>
       <c r="I17">
-        <f t="shared" si="6"/>
-        <v>87000</v>
+        <f t="shared" si="4"/>
+        <v>446250</v>
       </c>
       <c r="J17">
-        <f t="shared" si="7"/>
-        <v>446250</v>
+        <f>(G17-H17)*0.19</f>
+        <v>58425.760000000002</v>
+      </c>
+      <c r="K17">
+        <f>G17-H17-IF(J17&gt;0,J17,0)</f>
+        <v>249078.24</v>
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>39280.22</v>
+        <v>74723.471999999994</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>167457.78</v>
+        <v>174354.76799999998</v>
       </c>
       <c r="N17">
-        <f t="shared" si="2"/>
-        <v>50237.333999999995</v>
-      </c>
-      <c r="O17">
-        <f t="shared" si="3"/>
-        <v>117220.446</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="4"/>
-        <v>-329029.554</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M17-I17</f>
+        <v>-271895.23200000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="C18">
         <f>B17*0.1</f>
-        <v>1100</v>
+        <v>1300</v>
       </c>
       <c r="E18">
-        <f t="shared" si="5"/>
-        <v>69760</v>
+        <f t="shared" si="2"/>
+        <v>81280</v>
       </c>
       <c r="F18">
-        <f t="shared" si="9"/>
-        <v>2250</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G18">
+        <f>SUM(E$7:E18,F$7:F18)</f>
+        <v>482834</v>
       </c>
       <c r="H18">
-        <f>SUM(E$7:E18,F$7:F18)</f>
-        <v>365748</v>
+        <f t="shared" si="3"/>
+        <v>96000</v>
       </c>
       <c r="I18">
-        <f t="shared" si="6"/>
-        <v>90000</v>
+        <f t="shared" si="4"/>
+        <v>472500</v>
       </c>
       <c r="J18">
-        <f t="shared" si="7"/>
-        <v>472500</v>
+        <f>(G18-H18)*0.19</f>
+        <v>73498.460000000006</v>
+      </c>
+      <c r="K18">
+        <f>G18-H18-IF(J18&gt;0,J18,0)</f>
+        <v>313335.53999999998</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>52392.12</v>
+        <v>94000.661999999997</v>
       </c>
       <c r="M18">
         <f t="shared" si="1"/>
-        <v>223355.88</v>
+        <v>219334.87799999997</v>
       </c>
       <c r="N18">
-        <f t="shared" si="2"/>
-        <v>67006.763999999996</v>
-      </c>
-      <c r="O18">
-        <f t="shared" si="3"/>
-        <v>156349.11600000001</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="4"/>
-        <v>-316150.88399999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M18-I18</f>
+        <v>-253165.12200000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19">
-        <v>13000</v>
+        <v>15000</v>
       </c>
       <c r="C19">
-        <f t="shared" si="8"/>
-        <v>1200</v>
+        <f t="shared" si="5"/>
+        <v>1400</v>
       </c>
       <c r="E19">
-        <f t="shared" si="5"/>
-        <v>75520</v>
+        <f t="shared" si="2"/>
+        <v>87040</v>
       </c>
       <c r="F19">
-        <f>(C19-C18)*$B$3</f>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G19">
+        <f>SUM(E$7:E19,F$7:F19)</f>
+        <v>570924</v>
       </c>
       <c r="H19">
-        <f>SUM(E$7:E19,F$7:F19)</f>
-        <v>442768</v>
+        <f>H18+H$2+5000</f>
+        <v>104000</v>
       </c>
       <c r="I19">
-        <f>I18+I$2+5000</f>
-        <v>98000</v>
+        <f t="shared" si="4"/>
+        <v>498750</v>
       </c>
       <c r="J19">
-        <f t="shared" si="7"/>
-        <v>498750</v>
+        <f>(G19-H19)*0.19</f>
+        <v>88715.56</v>
+      </c>
+      <c r="K19">
+        <f>G19-H19-IF(J19&gt;0,J19,0)</f>
+        <v>378208.44</v>
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>65505.919999999998</v>
+        <v>113462.53199999999</v>
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>279262.08000000002</v>
+        <v>264745.908</v>
       </c>
       <c r="N19">
-        <f t="shared" si="2"/>
-        <v>83778.623999999996</v>
-      </c>
-      <c r="O19">
-        <f t="shared" si="3"/>
-        <v>195483.45600000001</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="4"/>
-        <v>-303266.54399999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M19-I19</f>
+        <v>-234004.092</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20">
-        <v>14000</v>
+        <v>16000</v>
       </c>
       <c r="C20">
-        <f t="shared" si="8"/>
-        <v>1300</v>
+        <f t="shared" si="5"/>
+        <v>1500</v>
       </c>
       <c r="E20">
-        <f t="shared" si="5"/>
-        <v>81280</v>
+        <f t="shared" si="2"/>
+        <v>92800</v>
       </c>
       <c r="F20">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G20">
+        <f>SUM(E$7:E20,F$7:F20)</f>
+        <v>664774</v>
       </c>
       <c r="H20">
-        <f>SUM(E$7:E20,F$7:F20)</f>
-        <v>525548</v>
+        <f t="shared" si="3"/>
+        <v>107000</v>
       </c>
       <c r="I20">
-        <f t="shared" si="6"/>
-        <v>101000</v>
+        <f t="shared" si="4"/>
+        <v>525000</v>
       </c>
       <c r="J20">
-        <f t="shared" si="7"/>
-        <v>525000</v>
+        <f>(G20-H20)*0.19</f>
+        <v>105977.06</v>
+      </c>
+      <c r="K20">
+        <f>G20-H20-IF(J20&gt;0,J20,0)</f>
+        <v>451796.94</v>
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>80664.12</v>
+        <v>135539.08199999999</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>343883.88</v>
+        <v>316257.85800000001</v>
       </c>
       <c r="N20">
-        <f t="shared" si="2"/>
-        <v>103165.164</v>
-      </c>
-      <c r="O20">
-        <f t="shared" si="3"/>
-        <v>240718.71600000001</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="4"/>
-        <v>-284281.28399999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M20-I20</f>
+        <v>-208742.14199999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21">
-        <v>15000</v>
+        <v>17000</v>
       </c>
       <c r="C21">
-        <f t="shared" si="8"/>
-        <v>1400</v>
+        <f t="shared" si="5"/>
+        <v>1600</v>
       </c>
       <c r="E21">
-        <f t="shared" si="5"/>
-        <v>87040</v>
+        <f t="shared" si="2"/>
+        <v>98560</v>
       </c>
       <c r="F21">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G21">
+        <f>SUM(E$7:E21,F$7:F21)</f>
+        <v>764384</v>
       </c>
       <c r="H21">
-        <f>SUM(E$7:E21,F$7:F21)</f>
-        <v>614088</v>
+        <f t="shared" si="3"/>
+        <v>110000</v>
       </c>
       <c r="I21">
-        <f t="shared" si="6"/>
-        <v>104000</v>
+        <f t="shared" si="4"/>
+        <v>551250</v>
       </c>
       <c r="J21">
-        <f t="shared" si="7"/>
-        <v>551250</v>
+        <f>(G21-H21)*0.19</f>
+        <v>124332.96</v>
+      </c>
+      <c r="K21">
+        <f>G21-H21-IF(J21&gt;0,J21,0)</f>
+        <v>530051.04</v>
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>96916.72</v>
+        <v>159015.31200000001</v>
       </c>
       <c r="M21">
         <f t="shared" si="1"/>
-        <v>413171.28</v>
+        <v>371035.728</v>
       </c>
       <c r="N21">
-        <f t="shared" si="2"/>
-        <v>123951.38400000001</v>
-      </c>
-      <c r="O21">
-        <f t="shared" si="3"/>
-        <v>289219.89600000001</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="4"/>
-        <v>-262030.10399999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M21-I21</f>
+        <v>-180214.272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22">
-        <v>16000</v>
+        <v>18000</v>
       </c>
       <c r="C22">
-        <f t="shared" si="8"/>
-        <v>1500</v>
+        <f t="shared" si="5"/>
+        <v>1700</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
-        <v>92800</v>
+        <f t="shared" si="2"/>
+        <v>104320</v>
       </c>
       <c r="F22">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G22">
+        <f>SUM(E$7:E22,F$7:F22)</f>
+        <v>869754</v>
       </c>
       <c r="H22">
-        <f>SUM(E$7:E22,F$7:F22)</f>
-        <v>708388</v>
+        <f t="shared" si="3"/>
+        <v>113000</v>
       </c>
       <c r="I22">
-        <f t="shared" si="6"/>
-        <v>107000</v>
+        <f t="shared" si="4"/>
+        <v>577500</v>
       </c>
       <c r="J22">
-        <f t="shared" si="7"/>
-        <v>577500</v>
+        <f>(G22-H22)*0.19</f>
+        <v>143783.26</v>
+      </c>
+      <c r="K22">
+        <f>G22-H22-IF(J22&gt;0,J22,0)</f>
+        <v>612970.74</v>
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>114263.72</v>
+        <v>183891.22199999998</v>
       </c>
       <c r="M22">
         <f t="shared" si="1"/>
-        <v>487124.28</v>
+        <v>429079.51800000004</v>
       </c>
       <c r="N22">
-        <f t="shared" si="2"/>
-        <v>146137.28400000001</v>
-      </c>
-      <c r="O22">
-        <f t="shared" si="3"/>
-        <v>340986.99600000004</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="4"/>
-        <v>-236513.00399999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M22-I22</f>
+        <v>-148420.48199999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23">
-        <v>17000</v>
+        <v>19000</v>
       </c>
       <c r="C23">
-        <f t="shared" si="8"/>
-        <v>1600</v>
+        <f t="shared" si="5"/>
+        <v>1800</v>
       </c>
       <c r="E23">
-        <f t="shared" si="5"/>
-        <v>98560</v>
+        <f t="shared" si="2"/>
+        <v>110080</v>
       </c>
       <c r="F23">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G23">
+        <f>SUM(E$7:E23,F$7:F23)</f>
+        <v>980884</v>
       </c>
       <c r="H23">
-        <f>SUM(E$7:E23,F$7:F23)</f>
-        <v>808448</v>
+        <f t="shared" si="3"/>
+        <v>116000</v>
       </c>
       <c r="I23">
-        <f t="shared" si="6"/>
-        <v>110000</v>
+        <f t="shared" si="4"/>
+        <v>603750</v>
       </c>
       <c r="J23">
-        <f t="shared" si="7"/>
-        <v>603750</v>
+        <f>(G23-H23)*0.19</f>
+        <v>164327.96</v>
+      </c>
+      <c r="K23">
+        <f>G23-H23-IF(J23&gt;0,J23,0)</f>
+        <v>700556.04</v>
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>132705.12</v>
+        <v>210166.81200000001</v>
       </c>
       <c r="M23">
         <f t="shared" si="1"/>
-        <v>565742.88</v>
+        <v>490389.228</v>
       </c>
       <c r="N23">
-        <f t="shared" si="2"/>
-        <v>169722.864</v>
-      </c>
-      <c r="O23">
-        <f t="shared" si="3"/>
-        <v>396020.016</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="4"/>
-        <v>-207729.984</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M23-I23</f>
+        <v>-113360.772</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24">
-        <v>18000</v>
+        <v>20000</v>
       </c>
       <c r="C24">
-        <f t="shared" si="8"/>
-        <v>1700</v>
+        <f t="shared" si="5"/>
+        <v>1900</v>
       </c>
       <c r="E24">
-        <f t="shared" si="5"/>
-        <v>104320</v>
+        <f t="shared" si="2"/>
+        <v>115840</v>
       </c>
       <c r="F24">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G24">
+        <f>SUM(E$7:E24,F$7:F24)</f>
+        <v>1097774</v>
       </c>
       <c r="H24">
-        <f>SUM(E$7:E24,F$7:F24)</f>
-        <v>914268</v>
+        <f t="shared" si="3"/>
+        <v>119000</v>
       </c>
       <c r="I24">
-        <f t="shared" si="6"/>
-        <v>113000</v>
+        <f t="shared" si="4"/>
+        <v>630000</v>
       </c>
       <c r="J24">
-        <f t="shared" si="7"/>
-        <v>630000</v>
+        <f>(G24-H24)*0.19</f>
+        <v>185967.06</v>
+      </c>
+      <c r="K24">
+        <f>G24-H24-IF(J24&gt;0,J24,0)</f>
+        <v>792806.94</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>152240.92000000001</v>
+        <v>237842.08199999997</v>
       </c>
       <c r="M24">
         <f t="shared" si="1"/>
-        <v>649027.07999999996</v>
+        <v>554964.85800000001</v>
       </c>
       <c r="N24">
-        <f t="shared" si="2"/>
-        <v>194708.12399999998</v>
-      </c>
-      <c r="O24">
-        <f t="shared" si="3"/>
-        <v>454318.95600000001</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="4"/>
-        <v>-175681.04399999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M24-I24</f>
+        <v>-75035.141999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25">
-        <v>19000</v>
+        <v>21000</v>
       </c>
       <c r="C25">
-        <f t="shared" si="8"/>
-        <v>1800</v>
+        <f t="shared" si="5"/>
+        <v>2000</v>
       </c>
       <c r="E25">
-        <f t="shared" si="5"/>
-        <v>110080</v>
+        <f t="shared" si="2"/>
+        <v>121600</v>
       </c>
       <c r="F25">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G25">
+        <f>SUM(E$7:E25,F$7:F25)</f>
+        <v>1220424</v>
       </c>
       <c r="H25">
-        <f>SUM(E$7:E25,F$7:F25)</f>
-        <v>1025848</v>
+        <f t="shared" si="3"/>
+        <v>122000</v>
       </c>
       <c r="I25">
-        <f t="shared" si="6"/>
-        <v>116000</v>
+        <f t="shared" si="4"/>
+        <v>656250</v>
       </c>
       <c r="J25">
-        <f t="shared" si="7"/>
-        <v>656250</v>
+        <f>(G25-H25)*0.19</f>
+        <v>208700.56</v>
+      </c>
+      <c r="K25">
+        <f>G25-H25-IF(J25&gt;0,J25,0)</f>
+        <v>889723.44</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>172871.12</v>
+        <v>266917.03199999995</v>
       </c>
       <c r="M25">
         <f t="shared" si="1"/>
-        <v>736976.88</v>
+        <v>622806.40800000005</v>
       </c>
       <c r="N25">
-        <f t="shared" si="2"/>
-        <v>221093.06399999998</v>
-      </c>
-      <c r="O25">
-        <f t="shared" si="3"/>
-        <v>515883.81599999999</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="4"/>
-        <v>-140366.18400000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M25-I25</f>
+        <v>-33443.591999999946</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26">
-        <v>20000</v>
+        <v>22000</v>
       </c>
       <c r="C26">
-        <f t="shared" si="8"/>
-        <v>1900</v>
+        <f t="shared" si="5"/>
+        <v>2100</v>
       </c>
       <c r="E26">
-        <f t="shared" si="5"/>
-        <v>115840</v>
+        <f t="shared" si="2"/>
+        <v>127360</v>
       </c>
       <c r="F26">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G26">
+        <f>SUM(E$7:E26,F$7:F26)</f>
+        <v>1348834</v>
       </c>
       <c r="H26">
-        <f>SUM(E$7:E26,F$7:F26)</f>
-        <v>1143188</v>
+        <f t="shared" si="3"/>
+        <v>125000</v>
       </c>
       <c r="I26">
-        <f t="shared" si="6"/>
-        <v>119000</v>
+        <f t="shared" si="4"/>
+        <v>682500</v>
       </c>
       <c r="J26">
-        <f t="shared" si="7"/>
-        <v>682500</v>
+        <f>(G26-H26)*0.19</f>
+        <v>232528.46</v>
+      </c>
+      <c r="K26">
+        <f>G26-H26-IF(J26&gt;0,J26,0)</f>
+        <v>991305.54</v>
       </c>
       <c r="L26">
         <f t="shared" si="0"/>
-        <v>194595.72</v>
+        <v>297391.66200000001</v>
       </c>
       <c r="M26">
         <f t="shared" si="1"/>
-        <v>829592.28</v>
+        <v>693913.87800000003</v>
       </c>
       <c r="N26">
-        <f t="shared" si="2"/>
-        <v>248877.68400000001</v>
-      </c>
-      <c r="O26">
-        <f t="shared" si="3"/>
-        <v>580714.59600000002</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="4"/>
-        <v>-101785.40399999998</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M26-I26</f>
+        <v>11413.878000000026</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27">
-        <v>21000</v>
+        <v>23000</v>
       </c>
       <c r="C27">
-        <f t="shared" si="8"/>
-        <v>2000</v>
+        <f t="shared" si="5"/>
+        <v>2200</v>
       </c>
       <c r="E27">
-        <f t="shared" si="5"/>
-        <v>121600</v>
+        <f t="shared" si="2"/>
+        <v>133120</v>
       </c>
       <c r="F27">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G27">
+        <f>SUM(E$7:E27,F$7:F27)</f>
+        <v>1483004</v>
       </c>
       <c r="H27">
-        <f>SUM(E$7:E27,F$7:F27)</f>
-        <v>1266288</v>
+        <f t="shared" si="3"/>
+        <v>128000</v>
       </c>
       <c r="I27">
-        <f t="shared" si="6"/>
-        <v>122000</v>
+        <f t="shared" si="4"/>
+        <v>708750</v>
       </c>
       <c r="J27">
-        <f t="shared" si="7"/>
-        <v>708750</v>
+        <f>(G27-H27)*0.19</f>
+        <v>257450.76</v>
+      </c>
+      <c r="K27">
+        <f>G27-H27-IF(J27&gt;0,J27,0)</f>
+        <v>1097553.24</v>
       </c>
       <c r="L27">
         <f t="shared" si="0"/>
-        <v>217414.72</v>
+        <v>329265.97200000001</v>
       </c>
       <c r="M27">
         <f t="shared" si="1"/>
-        <v>926873.28</v>
+        <v>768287.26799999992</v>
       </c>
       <c r="N27">
-        <f t="shared" si="2"/>
-        <v>278061.984</v>
-      </c>
-      <c r="O27">
-        <f t="shared" si="3"/>
-        <v>648811.29600000009</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="4"/>
-        <v>-59938.703999999911</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M27-I27</f>
+        <v>59537.267999999924</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28">
-        <v>22000</v>
+        <v>24000</v>
       </c>
       <c r="C28">
-        <f t="shared" si="8"/>
-        <v>2100</v>
+        <f t="shared" si="5"/>
+        <v>2300</v>
       </c>
       <c r="E28">
-        <f t="shared" si="5"/>
-        <v>127360</v>
+        <f t="shared" si="2"/>
+        <v>138880</v>
       </c>
       <c r="F28">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G28">
+        <f>SUM(E$7:E28,F$7:F28)</f>
+        <v>1622934</v>
       </c>
       <c r="H28">
-        <f>SUM(E$7:E28,F$7:F28)</f>
-        <v>1395148</v>
+        <f t="shared" si="3"/>
+        <v>131000</v>
       </c>
       <c r="I28">
-        <f t="shared" si="6"/>
-        <v>125000</v>
+        <f t="shared" si="4"/>
+        <v>735000</v>
       </c>
       <c r="J28">
-        <f t="shared" si="7"/>
-        <v>735000</v>
+        <f>(G28-H28)*0.19</f>
+        <v>283467.46000000002</v>
+      </c>
+      <c r="K28">
+        <f>G28-H28-IF(J28&gt;0,J28,0)</f>
+        <v>1208466.54</v>
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>241328.12</v>
+        <v>362539.962</v>
       </c>
       <c r="M28">
         <f t="shared" si="1"/>
-        <v>1028819.88</v>
+        <v>845926.57799999998</v>
       </c>
       <c r="N28">
-        <f t="shared" si="2"/>
-        <v>308645.96399999998</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="3"/>
-        <v>720173.91599999997</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="4"/>
-        <v>-14826.084000000032</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <f>M28-I28</f>
+        <v>110926.57799999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29">
-        <v>23000</v>
+        <v>25000</v>
       </c>
       <c r="C29">
-        <f t="shared" si="8"/>
-        <v>2200</v>
+        <f t="shared" si="5"/>
+        <v>2400</v>
       </c>
       <c r="E29">
-        <f t="shared" si="5"/>
-        <v>133120</v>
+        <f t="shared" si="2"/>
+        <v>144640</v>
       </c>
       <c r="F29">
-        <f t="shared" si="9"/>
-        <v>1500</v>
+        <f t="shared" si="6"/>
+        <v>1050</v>
+      </c>
+      <c r="G29">
+        <f>SUM(E$7:E29,F$7:F29)</f>
+        <v>1768624</v>
       </c>
       <c r="H29">
-        <f>SUM(E$7:E29,F$7:F29)</f>
-        <v>1529768</v>
+        <f t="shared" si="3"/>
+        <v>134000</v>
       </c>
       <c r="I29">
-        <f t="shared" si="6"/>
-        <v>128000</v>
+        <f t="shared" si="4"/>
+        <v>761250</v>
       </c>
       <c r="J29">
-        <f t="shared" si="7"/>
-        <v>761250</v>
+        <f>(G29-H29)*0.19</f>
+        <v>310578.56</v>
+      </c>
+      <c r="K29">
+        <f>G29-H29-IF(J29&gt;0,J29,0)</f>
+        <v>1324045.44</v>
       </c>
       <c r="L29">
         <f t="shared" si="0"/>
-        <v>266335.92</v>
+        <v>397213.63199999998</v>
       </c>
       <c r="M29">
         <f t="shared" si="1"/>
-        <v>1135432.08</v>
+        <v>926831.80799999996</v>
       </c>
       <c r="N29">
-        <f t="shared" si="2"/>
-        <v>340629.62400000001</v>
-      </c>
-      <c r="O29">
-        <f t="shared" si="3"/>
-        <v>794802.45600000001</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="4"/>
-        <v>33552.456000000006</v>
+        <f>M29-I29</f>
+        <v>165581.80799999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>